<commit_message>
perskambinau suzinojau alaus rusis, dabar reik parengt alaus db ir sulinkinti
</commit_message>
<xml_diff>
--- a/marketing/kauno-barai.xlsx
+++ b/marketing/kauno-barai.xlsx
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">brands!$A$1:$D$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'kauno-barai'!$A$1:$H$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'kauno-barai'!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="333">
   <si>
     <t>Baras</t>
   </si>
@@ -556,9 +556,6 @@
     <t>Skliautas</t>
   </si>
   <si>
-    <t>37 206843</t>
-  </si>
-  <si>
     <t>http://www.skliautas.com</t>
   </si>
   <si>
@@ -733,18 +730,6 @@
     <t>(8 46) 228822</t>
   </si>
   <si>
-    <t>http://www.facebook.com/Libertypub</t>
-  </si>
-  <si>
-    <t>Putvinskio g. 48, Kaunas</t>
-  </si>
-  <si>
-    <t>Liberty pub</t>
-  </si>
-  <si>
-    <t>liberty_pub</t>
-  </si>
-  <si>
     <t>Laisvės al. 51A, Kaunas</t>
   </si>
   <si>
@@ -799,9 +784,6 @@
     <t>bernelius_smukle</t>
   </si>
   <si>
-    <t>+370~686 57 449;</t>
-  </si>
-  <si>
     <t>http://www.berneliusmukle.lt</t>
   </si>
   <si>
@@ -871,12 +853,6 @@
     <t>23.8874186</t>
   </si>
   <si>
-    <t>54.9006537</t>
-  </si>
-  <si>
-    <t>23.9134524</t>
-  </si>
-  <si>
     <t>54.8986509</t>
   </si>
   <si>
@@ -931,9 +907,6 @@
     <t>55.695725</t>
   </si>
   <si>
-    <t>\21.14999</t>
-  </si>
-  <si>
     <t>54.8973275</t>
   </si>
   <si>
@@ -962,13 +935,97 @@
   </si>
   <si>
     <t>23.9138872</t>
+  </si>
+  <si>
+    <t>"+370 686 57 449"</t>
+  </si>
+  <si>
+    <t>Vilniaus g. 13, Kaunas</t>
+  </si>
+  <si>
+    <t>http://www.shamrock.lt</t>
+  </si>
+  <si>
+    <t>Shamrock</t>
+  </si>
+  <si>
+    <t>shamrock</t>
+  </si>
+  <si>
+    <t>8 37 206843</t>
+  </si>
+  <si>
+    <t>kalnapilis grand, kozel tamsus, tucher baltas, samson tamsus, krushovec sviesus, utenos dark, heineken, svyturio baltijos</t>
+  </si>
+  <si>
+    <t>grimbergen tamsus/sviesus, svyturio extra/baltas/baltijos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heineken, chodovar tamsus, kanapinis tamsus, Volfas Engelmanas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">samson tamsus, erdinger baltas, Volfas Engelmanas </t>
+  </si>
+  <si>
+    <t>Volfas Engelmanas ,  sinkoriu, sinkoriu tamsusis, svyturio extra/baltas</t>
+  </si>
+  <si>
+    <t>Volfas Engelmanas, Heineken</t>
+  </si>
+  <si>
+    <t>Svyturio extra/baltas, grimbergen sviesus</t>
+  </si>
+  <si>
+    <t>Volfas Engelmanas, Kalnapilis grand, viklmerges sviesus</t>
+  </si>
+  <si>
+    <t>hoegaarden, grimbergen tamsus/sviesus</t>
+  </si>
+  <si>
+    <t>grimbergen tamsus/sviesus, birzu miezinis, birzu sirvenos, svyturio extra/baltas</t>
+  </si>
+  <si>
+    <t>54.8966339</t>
+  </si>
+  <si>
+    <t>23.8897413</t>
+  </si>
+  <si>
+    <t>21.131396</t>
+  </si>
+  <si>
+    <t>55.708564</t>
+  </si>
+  <si>
+    <t>21.14999</t>
+  </si>
+  <si>
+    <t>Svyturio extra/baltas, carlsberg, guiness</t>
+  </si>
+  <si>
+    <t>Šviesusis Gyvasis, Karamelinis Vyšnių, Juodasis Degintas, Kvietinis Medaus</t>
+  </si>
+  <si>
+    <t>Vilkmergės HBH</t>
+  </si>
+  <si>
+    <t>hbh juozo alus</t>
+  </si>
+  <si>
+    <t>svyturio extra, kalnapilio grand, kozel tamsus</t>
+  </si>
+  <si>
+    <t>Butautu Dvaro alus</t>
+  </si>
+  <si>
+    <t>Kozel tamsus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -999,6 +1056,12 @@
       <family val="2"/>
       <charset val="186"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1024,7 +1087,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1032,6 +1095,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1327,22 +1391,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1388,10 +1452,10 @@
         <v>161</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>24</v>
@@ -1414,10 +1478,10 @@
         <v>166</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1437,10 +1501,13 @@
         <v>168</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
+      </c>
+      <c r="H4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1460,10 +1527,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1477,151 +1547,169 @@
         <v>175</v>
       </c>
       <c r="D6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>179</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
+      </c>
+      <c r="H6" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>182</v>
       </c>
-      <c r="D7" t="s">
-        <v>183</v>
-      </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
+      </c>
+      <c r="H7" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
         <v>185</v>
       </c>
-      <c r="B8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" t="s">
-        <v>186</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" t="s">
         <v>191</v>
-      </c>
-      <c r="B9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" t="s">
-        <v>192</v>
       </c>
       <c r="D9">
         <v>868508662</v>
       </c>
       <c r="E9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
+      </c>
+      <c r="H9" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" t="s">
         <v>229</v>
       </c>
-      <c r="D10" t="s">
-        <v>230</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
+      </c>
+      <c r="H10" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" t="s">
         <v>240</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>239</v>
       </c>
-      <c r="C11" t="s">
-        <v>238</v>
-      </c>
-      <c r="D11">
-        <v>865760121</v>
-      </c>
-      <c r="E11" t="s">
-        <v>237</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
         <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1641,79 +1729,117 @@
         <v>248</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>307</v>
+        <v>300</v>
+      </c>
+      <c r="H13" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C14" t="s">
         <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>305</v>
       </c>
       <c r="E14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>309</v>
+        <v>278</v>
+      </c>
+      <c r="H14" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>256</v>
-      </c>
-      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15">
+        <v>37067993033</v>
+      </c>
+      <c r="E15" t="s">
         <v>259</v>
       </c>
-      <c r="E15" t="s">
-        <v>260</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
+      </c>
+      <c r="H15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="C16" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16">
-        <v>37067993033</v>
-      </c>
-      <c r="E16" t="s">
-        <v>265</v>
+        <v>306</v>
+      </c>
+      <c r="D16" s="7">
+        <v>864154100</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>307</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>287</v>
+        <v>321</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>288</v>
+        <v>322</v>
+      </c>
+      <c r="H16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="H19" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1721,210 +1847,218 @@
         <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>283</v>
       </c>
       <c r="D20" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>201</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H20" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s">
-        <v>291</v>
+        <v>206</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>290</v>
+        <v>325</v>
+      </c>
+      <c r="H21" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" t="s">
         <v>207</v>
       </c>
-      <c r="D22" t="s">
-        <v>206</v>
-      </c>
       <c r="E22" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>302</v>
+        <v>212</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>303</v>
+        <v>213</v>
+      </c>
+      <c r="H22" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C23" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
-      </c>
-      <c r="E23" t="s">
-        <v>209</v>
+        <v>216</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>213</v>
+        <v>284</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>214</v>
+        <v>285</v>
+      </c>
+      <c r="H23" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" t="s">
         <v>219</v>
       </c>
-      <c r="C24" t="s">
-        <v>216</v>
-      </c>
       <c r="D24" t="s">
-        <v>217</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
+      </c>
+      <c r="H24" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D25" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" t="s">
         <v>223</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C26" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D26" t="s">
-        <v>227</v>
-      </c>
-      <c r="E26" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>301</v>
+        <v>289</v>
+      </c>
+      <c r="H26" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>264</v>
-      </c>
-      <c r="B28" t="s">
-        <v>263</v>
-      </c>
-      <c r="C28" t="s">
-        <v>261</v>
-      </c>
-      <c r="D28" t="s">
-        <v>262</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="I32" t="s">
+        <v>291</v>
+      </c>
+      <c r="H27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="I31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="3:4">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+    <row r="43" spans="3:4">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H43"/>
+  <autoFilter ref="A1:H42"/>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E24" r:id="rId2"/>
+    <hyperlink ref="E23" r:id="rId2"/>
+    <hyperlink ref="E16" r:id="rId3" display="http://www.shamrock.lt/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>